<commit_message>
Coherent pytest files with new Template.xlsx file
Signed-off-by: JasonMendoza2008 <lhotteromain@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/pytest_dr13.xlsx
+++ b/tests/pytest_dr13.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7970923-2078-493F-A4DD-97614919FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C9BFA-8970-4592-8354-80F4AB267CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="False Negs" sheetId="2" r:id="rId1"/>
@@ -63,24 +63,6 @@
     <t>PRED_TEST</t>
   </si>
   <si>
-    <t>HLA A1_D</t>
-  </si>
-  <si>
-    <t>HLA A2_D</t>
-  </si>
-  <si>
-    <t>HLA B1_D</t>
-  </si>
-  <si>
-    <t>HLA B2_D</t>
-  </si>
-  <si>
-    <t>HLA C1_D</t>
-  </si>
-  <si>
-    <t>HLA C2_D</t>
-  </si>
-  <si>
     <t>DRB11_D</t>
   </si>
   <si>
@@ -93,24 +75,6 @@
     <t>DQB12_D</t>
   </si>
   <si>
-    <t>HLA A1_R</t>
-  </si>
-  <si>
-    <t>HLA A2_R</t>
-  </si>
-  <si>
-    <t>HLA B1_R</t>
-  </si>
-  <si>
-    <t>HLA B2_R</t>
-  </si>
-  <si>
-    <t>HLA C1_R</t>
-  </si>
-  <si>
-    <t>HLA C2_R</t>
-  </si>
-  <si>
     <t>DRB11_R</t>
   </si>
   <si>
@@ -130,6 +94,42 @@
   </si>
   <si>
     <t>DRB1*13:02</t>
+  </si>
+  <si>
+    <t>A1_D</t>
+  </si>
+  <si>
+    <t>A2_D</t>
+  </si>
+  <si>
+    <t>B1_D</t>
+  </si>
+  <si>
+    <t>B2_D</t>
+  </si>
+  <si>
+    <t>C1_D</t>
+  </si>
+  <si>
+    <t>C2_D</t>
+  </si>
+  <si>
+    <t>A1_R</t>
+  </si>
+  <si>
+    <t>A2_R</t>
+  </si>
+  <si>
+    <t>B1_R</t>
+  </si>
+  <si>
+    <t>B2_R</t>
+  </si>
+  <si>
+    <t>C1_R</t>
+  </si>
+  <si>
+    <t>C2_R</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,13 +220,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,12 +509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF2FF63-4C5E-4611-9E93-6C23063652A5}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.77734375" style="3"/>
-    <col min="3" max="16384" width="12.77734375" style="2"/>
+    <col min="1" max="16384" width="12.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -530,75 +526,74 @@
     </row>
     <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -618,10 +613,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>0</v>
@@ -648,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>0</v>
@@ -670,12 +665,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843CE29D-CE6F-46AA-B26F-0FC90401288F}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.77734375" style="3"/>
-    <col min="3" max="16384" width="12.77734375" style="2"/>
+    <col min="1" max="16384" width="12.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -688,74 +682,74 @@
     </row>
     <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
@@ -775,10 +769,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>0</v>
@@ -805,10 +799,10 @@
         <v>3</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>0</v>

</xml_diff>